<commit_message>
Deploy listing for simplified Bolivia and non simplified vector tiles for Burkina Faso
Updating deployment registry for new vector tile fomat country and Bolivia simplfied json,kml, csv for Bolivia
</commit_message>
<xml_diff>
--- a/Data/AWSDeploymentURLlist.xlsx
+++ b/Data/AWSDeploymentURLlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arusso\Documents\GitHub\mapservicedoc\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A9B630-8E2F-4325-944F-B6474B44D9FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117F3ABE-35FD-41A0-8810-7C7EB817EEE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="60" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="128">
   <si>
     <t>Date posted</t>
   </si>
@@ -367,6 +367,54 @@
   </si>
   <si>
     <t>COD_LBR_Admin2</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin0.geojson</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin0.topojson</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin0.kml</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin0.csv</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin1.geojson</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin1.topojson</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin1.kml</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin1.csv</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin2.geojson</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin2.topojson</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin2.kml</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin3.kml</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin3.geojson</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin3.topojson</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin3.csv</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/BOL/COD_BOL_Admin2.csv</t>
   </si>
 </sst>
 </file>
@@ -411,10 +459,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -726,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G61" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2709,7 +2763,7 @@
         <v>https://itos-humanitarian.s3.amazonaws.com/SEN/COD_SEN_Admin3.topojson</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" ref="G66:H86" si="5">$B66&amp;"/"&amp;$C66&amp;"/"&amp;$D66&amp;".kml"</f>
+        <f t="shared" ref="G66:G86" si="5">$B66&amp;"/"&amp;$C66&amp;"/"&amp;$D66&amp;".kml"</f>
         <v>https://itos-humanitarian.s3.amazonaws.com/SEN/COD_SEN_Admin3.kml</v>
       </c>
       <c r="H66" t="str">
@@ -2731,7 +2785,7 @@
         <v>92</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E98" si="6">$B67&amp;"/"&amp;$C67&amp;"/"&amp;$D67&amp;$E$1</f>
+        <f t="shared" ref="E67:E86" si="6">$B67&amp;"/"&amp;$C67&amp;"/"&amp;$D67&amp;$E$1</f>
         <v>https://itos-humanitarian.s3.amazonaws.com/TGO/COD_TGO_Admin0.geojson</v>
       </c>
       <c r="F67" t="str">
@@ -3294,24 +3348,114 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="2"/>
-      <c r="B87" s="1"/>
+      <c r="A87" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C87" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" t="s">
+        <v>34</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-      <c r="B88" s="1"/>
+      <c r="A88" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C88" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" t="s">
+        <v>35</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="B89" s="1"/>
+      <c r="A89" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" t="s">
+        <v>36</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="B90" s="1"/>
+      <c r="A90" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C90" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" t="s">
+        <v>37</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="1"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
@@ -3352,8 +3496,24 @@
     <hyperlink ref="B84" r:id="rId7" xr:uid="{D59D5EF5-1DB1-4D8F-834F-583D60613154}"/>
     <hyperlink ref="B85" r:id="rId8" xr:uid="{37B62042-A5CF-4557-B060-523DCB4197A1}"/>
     <hyperlink ref="B86" r:id="rId9" xr:uid="{E47AA050-0EED-4FD9-A781-FAC39635A3D3}"/>
+    <hyperlink ref="E87" r:id="rId10" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin0.geojson" xr:uid="{310BEB6F-3636-4AA8-B626-7B772A90BE20}"/>
+    <hyperlink ref="F87" r:id="rId11" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin0.topojson" xr:uid="{AB041C73-41AA-425F-AD92-177F6DB38170}"/>
+    <hyperlink ref="G87" r:id="rId12" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin0.kml" xr:uid="{76C730E8-840C-4A6A-9AC2-D90278B62265}"/>
+    <hyperlink ref="H87" r:id="rId13" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin0.csv" xr:uid="{260F23CB-0292-4D16-BD7A-3324DFF35DDD}"/>
+    <hyperlink ref="E88" r:id="rId14" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin1.geojson" xr:uid="{96E49D99-A7C9-4B84-80F7-4AE19A5C061B}"/>
+    <hyperlink ref="F88" r:id="rId15" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin1.topojson" xr:uid="{EFD450B4-4FDB-4F2B-B226-77220AEED683}"/>
+    <hyperlink ref="G88" r:id="rId16" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin1.kml" xr:uid="{4A4C4CED-2240-4CC7-B6FD-96C3DFEBDD55}"/>
+    <hyperlink ref="H88" r:id="rId17" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin1.csv" xr:uid="{5F568AAF-878C-4D11-AC06-9D579309286D}"/>
+    <hyperlink ref="E89" r:id="rId18" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin2.geojson" xr:uid="{3EDAE9D2-CB85-4B9A-AD1C-8C195DA00FA3}"/>
+    <hyperlink ref="F89" r:id="rId19" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin2.topojson" xr:uid="{E19336B7-2666-4B91-AD4F-9433D016590D}"/>
+    <hyperlink ref="G89" r:id="rId20" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin2.kml" xr:uid="{BA22687D-2B9A-4F9F-BCD2-0C96BB81CCEE}"/>
+    <hyperlink ref="G90" r:id="rId21" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin2.kml" xr:uid="{E70CDC57-9148-46F8-B0FD-E9977F51CE83}"/>
+    <hyperlink ref="H89" r:id="rId22" xr:uid="{6E671B0C-6484-47FA-9CD0-DC136B822D9A}"/>
+    <hyperlink ref="H90" r:id="rId23" xr:uid="{77882D5D-4C83-4492-9FA4-BE2629EB5769}"/>
+    <hyperlink ref="E90" r:id="rId24" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin3.geojson" xr:uid="{5E0CCCC5-A13F-448D-814E-CF4CF81A73F0}"/>
+    <hyperlink ref="F90" r:id="rId25" display="https://itos-humanitarian.s3.amazonaws.com/LKA/COD_LKA_Admin3.topojson" xr:uid="{A484E4CD-F1DF-4C35-B7B4-96CE8BBDCAF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Syria admin 0 and 2 in mbtiles
Syria now complete for all vector tiles formats
</commit_message>
<xml_diff>
--- a/Data/AWSDeploymentURLlist.xlsx
+++ b/Data/AWSDeploymentURLlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arusso.OS\Documents\GitHub\mapservicedoc\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C76B21D-FB6A-42DE-9E57-4EC778CBD0A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B182A7C8-0A2A-4940-A898-359ACBEB2382}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44360" yWindow="2250" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294960433" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294939146" uniqueCount="234">
   <si>
     <t>Base URL for AWS</t>
   </si>
@@ -764,6 +764,12 @@
   </si>
   <si>
     <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_SYR/Admin0-MBT/Admin0.mbtiles</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_SYR/Admin2-MBT/Admin2.mbtiles</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J133" sqref="J133"/>
+    <sheetView tabSelected="1" topLeftCell="I87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3964,6 +3970,9 @@
       <c r="I94" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="J94" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="K94" s="1" t="s">
         <v>211</v>
       </c>
@@ -4000,6 +4009,9 @@
       </c>
       <c r="I96" s="1" t="s">
         <v>149</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>213</v>
@@ -4690,9 +4702,11 @@
     <hyperlink ref="K131" r:id="rId118" xr:uid="{554C13A0-DEA3-4CD5-AA98-85FE4C2F138E}"/>
     <hyperlink ref="K132" r:id="rId119" xr:uid="{97969E1D-C98B-470C-9153-4A80D88F2024}"/>
     <hyperlink ref="K130" r:id="rId120" xr:uid="{A2F4596B-74A2-4551-A3E7-FE1AFFD01F71}"/>
+    <hyperlink ref="J94" r:id="rId121" xr:uid="{DC78C57A-75EC-4426-A8F3-BF413DBB42D0}"/>
+    <hyperlink ref="J96" r:id="rId122" xr:uid="{75066307-3E9B-43F3-BA1B-B0E74B5F58E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId121"/>
-  <legacyDrawing r:id="rId122"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId123"/>
+  <legacyDrawing r:id="rId124"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nic, COD and others
Nicaragua, Democratic Republic of Congo COD and others
</commit_message>
<xml_diff>
--- a/Data/AWSDeploymentURLlist.xlsx
+++ b/Data/AWSDeploymentURLlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arusso.OS\Documents\GitHub\mapservicedoc\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F715B8D-2977-4B85-BD79-0A9B052B5C3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5EC60D-EB92-4E33-8AB4-C9229F8B7E22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="3860" windowWidth="25600" windowHeight="13390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="271">
   <si>
     <t>Base URL for AWS</t>
   </si>
@@ -548,15 +548,6 @@
     <t>MNG</t>
   </si>
   <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_MNG/Admin0-MBT/Admin0.mbtiles</t>
   </si>
   <si>
@@ -620,114 +611,18 @@
     <t>Dynamic Vectortiles (ocha-dap/gisrestapi or PGRestAPI)</t>
   </si>
   <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_YEM/Admin3/metadata.json</t>
   </si>
   <si>
     <t>VEN</t>
   </si>
   <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/3/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/3/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_IRQ/Admin-MBT/Admin0.mbtiles</t>
   </si>
   <si>
     <t>GHA</t>
   </si>
   <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/3/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/3/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/3/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_SYR/Admin3-MBT/Admin3.mbtiles</t>
   </si>
   <si>
@@ -758,15 +653,6 @@
     <t>DZA</t>
   </si>
   <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_SYR/Admin0-MBT/Admin0.mbtiles</t>
   </si>
   <si>
@@ -836,15 +722,6 @@
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_KHM/Admin1-MBT/Admin1.mbtiles</t>
   </si>
   <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/0/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/1/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
-    <t>http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/2/{z}/{x}/{y}.pbf</t>
-  </si>
-  <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_KHM/Admin2-MBT/Admin2.mbtiles</t>
   </si>
   <si>
@@ -855,6 +732,156 @@
   </si>
   <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_SAU/Admin0-MBT/Admin0.mbtiles</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COD/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COD/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COD/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/3/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/3/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/3/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/3/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/3/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_COD/Admin0-MBT/Admin0.mbtiles</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_COD/Admin1-MBT/Admin1.mbtiles</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_YEM/Admin2-MBT/Admin2.mbtiles</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/NIC/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/NIC/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/NIC/versions/current/2/{z}/{x}/{y}.pbf</t>
   </si>
 </sst>
 </file>
@@ -1243,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J146" sqref="J146"/>
+    <sheetView tabSelected="1" topLeftCell="J111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K142" sqref="K142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1293,7 +1320,7 @@
         <v>144</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1775,6 +1802,12 @@
         <f t="shared" si="3"/>
         <v>https://itos-humanitarian.s3.amazonaws.com/COD/COD_COD_Admin0.csv</v>
       </c>
+      <c r="J17" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
@@ -1805,6 +1838,12 @@
         <f>$B18&amp;"/"&amp;$C18&amp;"/"&amp;$D18&amp;$H$1</f>
         <v>https://itos-humanitarian.s3.amazonaws.com/COD/COD_COD_Admin1.csv</v>
       </c>
+      <c r="J18" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
@@ -1835,6 +1874,9 @@
         <f t="shared" si="3"/>
         <v>https://itos-humanitarian.s3.amazonaws.com/COD/COD_COD_Admin2.csv</v>
       </c>
+      <c r="K19" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
@@ -2079,7 +2121,7 @@
         <v>132</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -2115,7 +2157,7 @@
         <v>133</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -2151,7 +2193,7 @@
         <v>134</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -2190,7 +2232,7 @@
         <v>138</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -2403,10 +2445,10 @@
         <v>https://itos-humanitarian.s3.amazonaws.com/IRQ/COD_IRQ_Admin0.csv</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -2439,10 +2481,10 @@
         <v>https://itos-humanitarian.s3.amazonaws.com/IRQ/COD_IRQ_Admin1.csv</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -2475,10 +2517,10 @@
         <v>https://itos-humanitarian.s3.amazonaws.com/IRQ/COD_IRQ_Admin2.csv</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -2511,10 +2553,10 @@
         <v>https://itos-humanitarian.s3.amazonaws.com/IRQ/COD_IRQ_Admin3.csv</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -3699,7 +3741,7 @@
         <v>152</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
@@ -3735,7 +3777,7 @@
         <v>151</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
@@ -3771,7 +3813,7 @@
         <v>155</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.35">
@@ -4056,10 +4098,10 @@
         <v>136</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>232</v>
+        <v>194</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
@@ -4076,10 +4118,10 @@
         <v>150</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
@@ -4096,10 +4138,10 @@
         <v>149</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
@@ -4113,13 +4155,13 @@
         <v>137</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
@@ -4136,10 +4178,10 @@
         <v>140</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
@@ -4155,8 +4197,11 @@
       <c r="I99" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="J99" t="s">
+        <v>215</v>
+      </c>
       <c r="K99" s="1" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
@@ -4170,10 +4215,13 @@
         <v>139</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
@@ -4187,10 +4235,10 @@
         <v>139</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
@@ -4207,7 +4255,7 @@
         <v>146</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>208</v>
+        <v>243</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
@@ -4224,7 +4272,7 @@
         <v>147</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.35">
@@ -4241,7 +4289,7 @@
         <v>148</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>210</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.35">
@@ -4298,10 +4346,10 @@
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>160</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.35">
@@ -4316,10 +4364,10 @@
       </c>
       <c r="I109" s="1"/>
       <c r="J109" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>161</v>
+        <v>247</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.35">
@@ -4334,10 +4382,10 @@
       </c>
       <c r="I110" s="1"/>
       <c r="J110" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>159</v>
+        <v>248</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.35">
@@ -4348,13 +4396,13 @@
         <v>98</v>
       </c>
       <c r="C111" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>183</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.35">
@@ -4365,13 +4413,13 @@
         <v>98</v>
       </c>
       <c r="C112" t="s">
+        <v>165</v>
+      </c>
+      <c r="J112" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J112" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="K112" s="1" t="s">
-        <v>184</v>
+        <v>250</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.35">
@@ -4382,13 +4430,13 @@
         <v>98</v>
       </c>
       <c r="C113" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>185</v>
+        <v>251</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.35">
@@ -4399,13 +4447,13 @@
         <v>98</v>
       </c>
       <c r="C114" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>189</v>
+        <v>252</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.35">
@@ -4416,10 +4464,10 @@
         <v>98</v>
       </c>
       <c r="C115" t="s">
+        <v>170</v>
+      </c>
+      <c r="J115" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.35">
@@ -4430,10 +4478,10 @@
         <v>98</v>
       </c>
       <c r="C116" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.35">
@@ -4444,10 +4492,10 @@
         <v>98</v>
       </c>
       <c r="C117" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.35">
@@ -4458,13 +4506,13 @@
         <v>98</v>
       </c>
       <c r="C118" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>190</v>
+        <v>253</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.35">
@@ -4475,13 +4523,13 @@
         <v>98</v>
       </c>
       <c r="C119" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>191</v>
+        <v>254</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.35">
@@ -4492,13 +4540,13 @@
         <v>98</v>
       </c>
       <c r="C120" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>188</v>
+        <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.35">
@@ -4509,10 +4557,10 @@
         <v>98</v>
       </c>
       <c r="C121" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.35">
@@ -4523,10 +4571,10 @@
         <v>98</v>
       </c>
       <c r="C122" t="s">
+        <v>181</v>
+      </c>
+      <c r="J122" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="J122" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.35">
@@ -4537,10 +4585,10 @@
         <v>98</v>
       </c>
       <c r="C123" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.35">
@@ -4551,10 +4599,10 @@
         <v>98</v>
       </c>
       <c r="C124" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>198</v>
+        <v>256</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.35">
@@ -4565,10 +4613,10 @@
         <v>98</v>
       </c>
       <c r="C125" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>199</v>
+        <v>257</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.35">
@@ -4579,10 +4627,10 @@
         <v>98</v>
       </c>
       <c r="C126" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>200</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.35">
@@ -4593,10 +4641,10 @@
         <v>98</v>
       </c>
       <c r="C127" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.35">
@@ -4607,10 +4655,10 @@
         <v>98</v>
       </c>
       <c r="C128" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
       <c r="J128" s="1"/>
     </row>
@@ -4622,10 +4670,10 @@
         <v>98</v>
       </c>
       <c r="C129" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="J129" s="1"/>
     </row>
@@ -4637,13 +4685,10 @@
         <v>98</v>
       </c>
       <c r="C130" t="s">
-        <v>228</v>
-      </c>
-      <c r="J130" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="K130" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="K130" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.35">
@@ -4654,10 +4699,13 @@
         <v>98</v>
       </c>
       <c r="C131" t="s">
-        <v>228</v>
+        <v>193</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.35">
@@ -4668,10 +4716,10 @@
         <v>98</v>
       </c>
       <c r="C132" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.35">
@@ -4682,13 +4730,16 @@
         <v>98</v>
       </c>
       <c r="C133" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>235</v>
+        <v>197</v>
+      </c>
+      <c r="K133" s="1" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.35">
@@ -4699,13 +4750,16 @@
         <v>98</v>
       </c>
       <c r="C134" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>247</v>
+        <v>209</v>
+      </c>
+      <c r="K134" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.35">
@@ -4716,13 +4770,16 @@
         <v>98</v>
       </c>
       <c r="C135" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>246</v>
+        <v>208</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.35">
@@ -4733,10 +4790,10 @@
         <v>98</v>
       </c>
       <c r="C136" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.35">
@@ -4747,10 +4804,10 @@
         <v>98</v>
       </c>
       <c r="C137" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.35">
@@ -4761,10 +4818,10 @@
         <v>98</v>
       </c>
       <c r="C138" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.35">
@@ -4775,10 +4832,10 @@
         <v>98</v>
       </c>
       <c r="C139" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.35">
@@ -4789,10 +4846,10 @@
         <v>98</v>
       </c>
       <c r="C140" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>243</v>
+        <v>205</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.35">
@@ -4803,10 +4860,10 @@
         <v>98</v>
       </c>
       <c r="C141" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.35">
@@ -4817,10 +4874,10 @@
         <v>98</v>
       </c>
       <c r="C142" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.35">
@@ -4831,13 +4888,13 @@
         <v>98</v>
       </c>
       <c r="C143" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.35">
@@ -4848,13 +4905,13 @@
         <v>98</v>
       </c>
       <c r="C144" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.35">
@@ -4865,13 +4922,13 @@
         <v>98</v>
       </c>
       <c r="C145" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>258</v>
+        <v>217</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.35">
@@ -4882,10 +4939,10 @@
         <v>98</v>
       </c>
       <c r="C146" t="s">
-        <v>260</v>
+        <v>219</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>261</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4962,43 +5019,43 @@
     <hyperlink ref="J115" r:id="rId70" xr:uid="{FFB1EB30-35D8-40FC-AC28-120E9D4EA50B}"/>
     <hyperlink ref="J119" r:id="rId71" xr:uid="{6E287DD5-4B61-4A5A-A23C-B0061E2B7385}"/>
     <hyperlink ref="J117" r:id="rId72" xr:uid="{18F2C76A-3AB8-4254-BF75-F4E008674394}"/>
-    <hyperlink ref="K108" r:id="rId73" xr:uid="{402CCA51-7F98-47D9-8829-B454DF1B89F7}"/>
-    <hyperlink ref="K109" r:id="rId74" xr:uid="{34F4E5E7-F503-4CA1-A494-6E942959B187}"/>
-    <hyperlink ref="K110" r:id="rId75" xr:uid="{8D267C7F-8E49-47A6-A308-CFF5CBF170C4}"/>
-    <hyperlink ref="K111" r:id="rId76" xr:uid="{3BD53969-2D37-4AF7-BF4D-05FEA5618AC8}"/>
-    <hyperlink ref="K112" r:id="rId77" xr:uid="{AD15FE32-7D55-40A9-A807-6406B928E011}"/>
-    <hyperlink ref="K113" r:id="rId78" xr:uid="{0CA86BB3-FA30-457C-85BC-6C4886A2D471}"/>
-    <hyperlink ref="K114" r:id="rId79" xr:uid="{7628FEFC-BC4F-4A27-8106-AE7DE93FEC84}"/>
-    <hyperlink ref="K119" r:id="rId80" xr:uid="{13FAF3D8-E262-4D69-950F-6EF92DD0DC73}"/>
-    <hyperlink ref="K120" r:id="rId81" xr:uid="{04536EB6-44A4-4E1B-B6FC-2A247BC2AF82}"/>
+    <hyperlink ref="K108" r:id="rId73" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{402CCA51-7F98-47D9-8829-B454DF1B89F7}"/>
+    <hyperlink ref="K109" r:id="rId74" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{34F4E5E7-F503-4CA1-A494-6E942959B187}"/>
+    <hyperlink ref="K110" r:id="rId75" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/MNG/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{8D267C7F-8E49-47A6-A308-CFF5CBF170C4}"/>
+    <hyperlink ref="K111" r:id="rId76" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{3BD53969-2D37-4AF7-BF4D-05FEA5618AC8}"/>
+    <hyperlink ref="K112" r:id="rId77" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{AD15FE32-7D55-40A9-A807-6406B928E011}"/>
+    <hyperlink ref="K113" r:id="rId78" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{0CA86BB3-FA30-457C-85BC-6C4886A2D471}"/>
+    <hyperlink ref="K114" r:id="rId79" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KGZ/versions/current/3/{z}/{x}/{y}.pbf" xr:uid="{7628FEFC-BC4F-4A27-8106-AE7DE93FEC84}"/>
+    <hyperlink ref="K119" r:id="rId80" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{13FAF3D8-E262-4D69-950F-6EF92DD0DC73}"/>
+    <hyperlink ref="K120" r:id="rId81" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{04536EB6-44A4-4E1B-B6FC-2A247BC2AF82}"/>
     <hyperlink ref="B101" r:id="rId82" xr:uid="{2EC1E14B-E486-42A0-AF48-8011901A29EA}"/>
     <hyperlink ref="I101" r:id="rId83" xr:uid="{99C2E917-1857-4F83-BD67-59B87C58482D}"/>
-    <hyperlink ref="K118" r:id="rId84" xr:uid="{93138F79-06FD-4F5C-94D6-142702BB72FF}"/>
-    <hyperlink ref="K27" r:id="rId85" xr:uid="{E337C9D7-016E-4D71-BE8D-384A8065FC13}"/>
-    <hyperlink ref="K28" r:id="rId86" xr:uid="{4E72D00A-4777-44EC-9AB7-E22DCDA85AA0}"/>
-    <hyperlink ref="K29" r:id="rId87" xr:uid="{A8C3F93F-2DB0-4D0A-9BD5-DC5F53E5D8CD}"/>
-    <hyperlink ref="K30" r:id="rId88" xr:uid="{426D28A6-A079-4817-8499-108EE733B7CA}"/>
-    <hyperlink ref="K125" r:id="rId89" xr:uid="{46C1E08E-6D9F-48DD-B267-6AD650890F54}"/>
-    <hyperlink ref="K126" r:id="rId90" xr:uid="{41905F37-9E79-4D28-9060-2B1DF1D1A7A6}"/>
-    <hyperlink ref="K124" r:id="rId91" xr:uid="{2ECDCAFC-0BA7-44A4-BC9C-A5412CEFB0B3}"/>
-    <hyperlink ref="K37" r:id="rId92" xr:uid="{773640F8-59E2-4CDC-A289-181E6CB1485A}"/>
-    <hyperlink ref="K38" r:id="rId93" xr:uid="{4FA22D46-F40C-4209-AD0E-2C29DB9E62B9}"/>
-    <hyperlink ref="K39" r:id="rId94" xr:uid="{0E936E58-B2FB-49E6-BAB4-77A8C880F1BD}"/>
-    <hyperlink ref="K40" r:id="rId95" xr:uid="{570A943D-3EDD-483D-A84A-1D06463044DF}"/>
-    <hyperlink ref="K80" r:id="rId96" xr:uid="{D2FDEFCA-1DA7-4F34-9CA9-AF1873AB81E0}"/>
-    <hyperlink ref="K81" r:id="rId97" xr:uid="{31177326-FA16-4819-AA76-2B8CA9E4489B}"/>
-    <hyperlink ref="K82" r:id="rId98" xr:uid="{676BA508-DF52-4E7A-822D-3F987C4CEA17}"/>
-    <hyperlink ref="K102" r:id="rId99" xr:uid="{7E7374A2-8F51-4023-BC0B-89218B35AB29}"/>
-    <hyperlink ref="K103" r:id="rId100" xr:uid="{6622811A-2E06-4F98-A93B-E126E4B41484}"/>
-    <hyperlink ref="K104" r:id="rId101" xr:uid="{B11ED906-3994-4C9C-A14A-7C0157AFF582}"/>
-    <hyperlink ref="K94" r:id="rId102" xr:uid="{9FF1B1BC-9C9D-4E19-B5A8-B5C1F2BA8782}"/>
-    <hyperlink ref="K95" r:id="rId103" xr:uid="{6D89302F-387C-4643-8AB5-158C91B068AB}"/>
-    <hyperlink ref="K96" r:id="rId104" xr:uid="{C3976E67-798E-4846-9730-9214C80D929F}"/>
-    <hyperlink ref="K97" r:id="rId105" xr:uid="{539127CF-D395-499F-9665-8766742FFAB2}"/>
-    <hyperlink ref="K98" r:id="rId106" xr:uid="{3334DDD0-5A3E-4445-9E05-5CC58345D6B7}"/>
-    <hyperlink ref="K99" r:id="rId107" xr:uid="{CCF9E870-A156-414E-A854-6B634357C424}"/>
-    <hyperlink ref="K100" r:id="rId108" xr:uid="{0E3D8422-7852-46C7-80B2-679C00ED4DC5}"/>
-    <hyperlink ref="K101" r:id="rId109" xr:uid="{90900B07-2349-47D8-A137-4A9A168BEF8E}"/>
+    <hyperlink ref="K118" r:id="rId84" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/COL/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{93138F79-06FD-4F5C-94D6-142702BB72FF}"/>
+    <hyperlink ref="K27" r:id="rId85" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{E337C9D7-016E-4D71-BE8D-384A8065FC13}"/>
+    <hyperlink ref="K28" r:id="rId86" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{4E72D00A-4777-44EC-9AB7-E22DCDA85AA0}"/>
+    <hyperlink ref="K29" r:id="rId87" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{A8C3F93F-2DB0-4D0A-9BD5-DC5F53E5D8CD}"/>
+    <hyperlink ref="K30" r:id="rId88" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/ETH/versions/current/3/{z}/{x}/{y}.pbf" xr:uid="{426D28A6-A079-4817-8499-108EE733B7CA}"/>
+    <hyperlink ref="K125" r:id="rId89" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{46C1E08E-6D9F-48DD-B267-6AD650890F54}"/>
+    <hyperlink ref="K126" r:id="rId90" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{41905F37-9E79-4D28-9060-2B1DF1D1A7A6}"/>
+    <hyperlink ref="K124" r:id="rId91" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/GHA/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{2ECDCAFC-0BA7-44A4-BC9C-A5412CEFB0B3}"/>
+    <hyperlink ref="K37" r:id="rId92" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{773640F8-59E2-4CDC-A289-181E6CB1485A}"/>
+    <hyperlink ref="K38" r:id="rId93" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{4FA22D46-F40C-4209-AD0E-2C29DB9E62B9}"/>
+    <hyperlink ref="K39" r:id="rId94" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{0E936E58-B2FB-49E6-BAB4-77A8C880F1BD}"/>
+    <hyperlink ref="K40" r:id="rId95" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/IRQ/versions/current/3/{z}/{x}/{y}.pbf" xr:uid="{570A943D-3EDD-483D-A84A-1D06463044DF}"/>
+    <hyperlink ref="K80" r:id="rId96" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{D2FDEFCA-1DA7-4F34-9CA9-AF1873AB81E0}"/>
+    <hyperlink ref="K81" r:id="rId97" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{31177326-FA16-4819-AA76-2B8CA9E4489B}"/>
+    <hyperlink ref="K82" r:id="rId98" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/LBR/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{676BA508-DF52-4E7A-822D-3F987C4CEA17}"/>
+    <hyperlink ref="K102" r:id="rId99" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{7E7374A2-8F51-4023-BC0B-89218B35AB29}"/>
+    <hyperlink ref="K103" r:id="rId100" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{6622811A-2E06-4F98-A93B-E126E4B41484}"/>
+    <hyperlink ref="K104" r:id="rId101" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SOM/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{B11ED906-3994-4C9C-A14A-7C0157AFF582}"/>
+    <hyperlink ref="K94" r:id="rId102" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{9FF1B1BC-9C9D-4E19-B5A8-B5C1F2BA8782}"/>
+    <hyperlink ref="K95" r:id="rId103" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{6D89302F-387C-4643-8AB5-158C91B068AB}"/>
+    <hyperlink ref="K96" r:id="rId104" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{C3976E67-798E-4846-9730-9214C80D929F}"/>
+    <hyperlink ref="K97" r:id="rId105" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/SYR/versions/current/3/{z}/{x}/{y}.pbf" xr:uid="{539127CF-D395-499F-9665-8766742FFAB2}"/>
+    <hyperlink ref="K98" r:id="rId106" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{3334DDD0-5A3E-4445-9E05-5CC58345D6B7}"/>
+    <hyperlink ref="K99" r:id="rId107" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{CCF9E870-A156-414E-A854-6B634357C424}"/>
+    <hyperlink ref="K100" r:id="rId108" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{0E3D8422-7852-46C7-80B2-679C00ED4DC5}"/>
+    <hyperlink ref="K101" r:id="rId109" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/YEM/versions/current/3/{z}/{x}/{y}.pbf" xr:uid="{90900B07-2349-47D8-A137-4A9A168BEF8E}"/>
     <hyperlink ref="J97" r:id="rId110" xr:uid="{9F8F9CD0-E481-4585-B5C1-56D66B537054}"/>
     <hyperlink ref="J123" r:id="rId111" xr:uid="{9DF99CEA-FA5A-4A14-8718-DFF4AFC71F72}"/>
     <hyperlink ref="J122" r:id="rId112" xr:uid="{9FD0A0C6-8B1F-4661-B51C-FEB9AE37B405}"/>
@@ -5007,9 +5064,9 @@
     <hyperlink ref="I129" r:id="rId115" xr:uid="{1D18298C-5748-4B8D-A409-8DF4A2B10270}"/>
     <hyperlink ref="I128" r:id="rId116" xr:uid="{73EFE52F-67BF-4688-8A3C-95F5BAF89D0E}"/>
     <hyperlink ref="I127" r:id="rId117" xr:uid="{813F65DE-0FB0-400D-ABBA-AE8427594C11}"/>
-    <hyperlink ref="K131" r:id="rId118" xr:uid="{554C13A0-DEA3-4CD5-AA98-85FE4C2F138E}"/>
-    <hyperlink ref="K132" r:id="rId119" xr:uid="{97969E1D-C98B-470C-9153-4A80D88F2024}"/>
-    <hyperlink ref="K130" r:id="rId120" xr:uid="{A2F4596B-74A2-4551-A3E7-FE1AFFD01F71}"/>
+    <hyperlink ref="K131" r:id="rId118" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{554C13A0-DEA3-4CD5-AA98-85FE4C2F138E}"/>
+    <hyperlink ref="K132" r:id="rId119" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{97969E1D-C98B-470C-9153-4A80D88F2024}"/>
+    <hyperlink ref="K130" r:id="rId120" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/DZA/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{A2F4596B-74A2-4551-A3E7-FE1AFFD01F71}"/>
     <hyperlink ref="J94" r:id="rId121" xr:uid="{DC78C57A-75EC-4426-A8F3-BF413DBB42D0}"/>
     <hyperlink ref="J96" r:id="rId122" xr:uid="{75066307-3E9B-43F3-BA1B-B0E74B5F58E6}"/>
     <hyperlink ref="J133" r:id="rId123" xr:uid="{3D5A927C-F34B-4B4C-BD09-A6537A00D1DC}"/>
@@ -5029,15 +5086,24 @@
     <hyperlink ref="J118" r:id="rId137" xr:uid="{3FD6418A-59A2-4D05-A7EB-B901B342FB6A}"/>
     <hyperlink ref="J98" r:id="rId138" xr:uid="{26770539-66D6-44FC-9503-2D2AE2154AE9}"/>
     <hyperlink ref="J144" r:id="rId139" xr:uid="{3293E3FD-AA84-4E3C-A9B2-98937D1BE16B}"/>
-    <hyperlink ref="K143" r:id="rId140" xr:uid="{2E962C8A-18CE-4B3C-828F-FE9AA2273475}"/>
-    <hyperlink ref="K144" r:id="rId141" xr:uid="{F34676E9-097B-459E-9FEC-C7532623DBFC}"/>
-    <hyperlink ref="K145" r:id="rId142" xr:uid="{FF060BDC-822F-4E5D-AA16-4B9904050AD2}"/>
+    <hyperlink ref="K143" r:id="rId140" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/0/{z}/{x}/{y}.pbf" xr:uid="{2E962C8A-18CE-4B3C-828F-FE9AA2273475}"/>
+    <hyperlink ref="K144" r:id="rId141" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/1/{z}/{x}/{y}.pbf" xr:uid="{F34676E9-097B-459E-9FEC-C7532623DBFC}"/>
+    <hyperlink ref="K145" r:id="rId142" display="http://beta.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/KHM/versions/current/2/{z}/{x}/{y}.pbf" xr:uid="{FF060BDC-822F-4E5D-AA16-4B9904050AD2}"/>
     <hyperlink ref="J145" r:id="rId143" xr:uid="{77F9D874-BCD2-49CB-8F54-0A9E182FB66E}"/>
-    <hyperlink ref="J130" r:id="rId144" xr:uid="{6D5ED7A7-6A8E-4D1F-8C21-BB5EB8CF7254}"/>
+    <hyperlink ref="J131" r:id="rId144" xr:uid="{6D5ED7A7-6A8E-4D1F-8C21-BB5EB8CF7254}"/>
     <hyperlink ref="J146" r:id="rId145" xr:uid="{9681BF45-1848-42D9-BFCE-706E6B2FB901}"/>
+    <hyperlink ref="K17" r:id="rId146" xr:uid="{B75C7242-642D-47AC-A4ED-EDEF7AC1AE21}"/>
+    <hyperlink ref="K18" r:id="rId147" xr:uid="{D9C052D1-969F-4965-A776-362144A9A7EA}"/>
+    <hyperlink ref="K19" r:id="rId148" xr:uid="{D781FC18-82A0-40EE-88CF-8BDAFE359D3E}"/>
+    <hyperlink ref="J17" r:id="rId149" xr:uid="{7537EE23-4C61-4571-941C-3731658B1BA7}"/>
+    <hyperlink ref="J18" r:id="rId150" xr:uid="{372BB3E0-E07E-4961-9EE6-9868B794E285}"/>
+    <hyperlink ref="J100" r:id="rId151" xr:uid="{2261F0C3-678C-42AE-B307-81D491337945}"/>
+    <hyperlink ref="K134" r:id="rId152" xr:uid="{B6964586-A914-40B5-878B-6530BC25DB48}"/>
+    <hyperlink ref="K135" r:id="rId153" xr:uid="{CCA159A9-92A4-4AA0-AC7A-70352B2C47B1}"/>
+    <hyperlink ref="K133" r:id="rId154" xr:uid="{C3979E1D-98F9-4789-A6A1-222E8B260C0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId146"/>
-  <legacyDrawing r:id="rId147"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId155"/>
+  <legacyDrawing r:id="rId156"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Timor-Leste and Mexico updates
Timor-Leste and Mexico updates
</commit_message>
<xml_diff>
--- a/Data/AWSDeploymentURLlist.xlsx
+++ b/Data/AWSDeploymentURLlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arusso.OS\Documents\GitHub\mapservicedoc\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D759F76-B600-42EB-B871-79EF5AEBC266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30AC13C-47B6-42FD-9C72-DCE2DE87AEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8250" yWindow="3560" windowWidth="25600" windowHeight="13390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8590" yWindow="3900" windowWidth="25600" windowHeight="13390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="311">
   <si>
     <t>Base URL for AWS</t>
   </si>
@@ -977,6 +977,30 @@
   </si>
   <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_GHA/Admin2-MBT/Admin2.mbtiles</t>
+  </si>
+  <si>
+    <t>TLS</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/TLS/versions/current/0/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/TLS/versions/current/1/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>http://apps.itos.uga.edu/CODV2API/api/v1/Themes/cod-ab/locations/TLS/versions/current/2/{z}/{x}/{y}.pbf</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_TLS/Admin0-MBT/Admin0.mbtiles</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_TLS/Admin1-MBT/Admin1.mbtiles</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_TLS/Admin2-MBT/Admin2.mbtiles</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_TLS/Admin3-MBT/Admin3.mbtiles</t>
   </si>
 </sst>
 </file>
@@ -1363,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K154"/>
+  <dimension ref="A1:K158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J126" sqref="J126"/>
+    <sheetView tabSelected="1" topLeftCell="J131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J158" sqref="J158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5211,6 +5235,74 @@
       </c>
       <c r="K154" s="1" t="s">
         <v>301</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A155" s="2">
+        <v>44376</v>
+      </c>
+      <c r="B155" t="s">
+        <v>98</v>
+      </c>
+      <c r="C155" t="s">
+        <v>303</v>
+      </c>
+      <c r="J155" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="K155" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A156" s="2">
+        <v>44376</v>
+      </c>
+      <c r="B156" t="s">
+        <v>98</v>
+      </c>
+      <c r="C156" t="s">
+        <v>303</v>
+      </c>
+      <c r="J156" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="K156" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A157" s="2">
+        <v>44376</v>
+      </c>
+      <c r="B157" t="s">
+        <v>98</v>
+      </c>
+      <c r="C157" t="s">
+        <v>303</v>
+      </c>
+      <c r="J157" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="K157" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A158" s="2">
+        <v>44376</v>
+      </c>
+      <c r="B158" t="s">
+        <v>98</v>
+      </c>
+      <c r="C158" t="s">
+        <v>303</v>
+      </c>
+      <c r="J158" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="K158" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -5400,9 +5492,17 @@
     <hyperlink ref="K153" r:id="rId183" xr:uid="{E86548D3-433B-49EB-93E6-5BFB4D6A3806}"/>
     <hyperlink ref="K154" r:id="rId184" xr:uid="{B3376FC1-EC1A-489E-9405-CA926EC1A7CB}"/>
     <hyperlink ref="J126" r:id="rId185" xr:uid="{F28E3EB8-39FE-448C-B46C-718A1A672592}"/>
+    <hyperlink ref="K155" r:id="rId186" xr:uid="{3C97D69F-DC60-42C9-B95A-6396E9970D05}"/>
+    <hyperlink ref="K156" r:id="rId187" xr:uid="{5E5EB37F-1134-49F2-BE0A-4DED80104A41}"/>
+    <hyperlink ref="K157" r:id="rId188" xr:uid="{7E50CB05-C5EF-42CE-9BFE-EF3148E8B05E}"/>
+    <hyperlink ref="K158" r:id="rId189" xr:uid="{9D804933-7111-4A53-9CB7-457EE736C4BD}"/>
+    <hyperlink ref="J155" r:id="rId190" xr:uid="{C486CB56-149F-4895-867A-BD478B0D7C6C}"/>
+    <hyperlink ref="J156" r:id="rId191" xr:uid="{36556C04-474E-4CCE-939B-1E43366EB41B}"/>
+    <hyperlink ref="J157" r:id="rId192" xr:uid="{48791F54-3519-4904-AE5D-433DD27D12E5}"/>
+    <hyperlink ref="J158" r:id="rId193" xr:uid="{9B9CD70E-80BB-476F-AFD2-67FC32A932E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId186"/>
-  <legacyDrawing r:id="rId187"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId194"/>
+  <legacyDrawing r:id="rId195"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up and update for hdx api changes
Remove data from scripts directory and remove copies. Update the scripts to run with the updated hdx api (hdx.api.configuration replacing hdx_configuration)
</commit_message>
<xml_diff>
--- a/Data/AWSDeploymentURLlist.xlsx
+++ b/Data/AWSDeploymentURLlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arusso.OS\Documents\GitHub\mapservicedoc\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FC9CBA-CDF1-4A47-AE19-5C0DDCE3EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2173891B-99B3-4355-A51D-CF1EDB68CEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1740" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="2150" windowWidth="28800" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="391">
   <si>
     <t>Base URL for AWS</t>
   </si>
@@ -1232,6 +1232,15 @@
   </si>
   <si>
     <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_MEX/South/Admin1/metadata.json</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_SEN/Admin1/metadata.json</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_SEN/Admin2/metadata.json</t>
+  </si>
+  <si>
+    <t>https://itos-humanitarian.s3.amazonaws.com/v1/VectorTile/COD_SEN/Admin3/metadata.json</t>
   </si>
 </sst>
 </file>
@@ -1621,8 +1630,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I189" sqref="I189"/>
+    <sheetView tabSelected="1" topLeftCell="H55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3650,6 +3659,9 @@
         <f t="shared" si="3"/>
         <v>https://itos-humanitarian.s3.amazonaws.com/SEN/COD_SEN_Admin1.csv</v>
       </c>
+      <c r="I64" s="1" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
@@ -3680,6 +3692,9 @@
         <f t="shared" si="3"/>
         <v>https://itos-humanitarian.s3.amazonaws.com/SEN/COD_SEN_Admin2.csv</v>
       </c>
+      <c r="I65" s="1" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
@@ -3709,6 +3724,9 @@
       <c r="H66" t="str">
         <f t="shared" si="3"/>
         <v>https://itos-humanitarian.s3.amazonaws.com/SEN/COD_SEN_Admin3.csv</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
@@ -6356,9 +6374,12 @@
     <hyperlink ref="I188" r:id="rId255" xr:uid="{3F68F38C-08A5-4223-8900-A7D3A0906360}"/>
     <hyperlink ref="I187" r:id="rId256" xr:uid="{0254502D-92AA-4BC4-A4CE-FA0D60EF7F41}"/>
     <hyperlink ref="I189" r:id="rId257" xr:uid="{4AFD224D-B35E-486E-A9F3-29F156533453}"/>
+    <hyperlink ref="I64" r:id="rId258" xr:uid="{5C160E81-E1EA-4EDB-A8EF-B7BF28774016}"/>
+    <hyperlink ref="I65" r:id="rId259" xr:uid="{73C7EB6C-71AE-40DF-8E01-B67F534D2E1B}"/>
+    <hyperlink ref="I66" r:id="rId260" xr:uid="{EB425AC1-51D5-4CA8-B78F-BE067B53A39B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId258"/>
-  <legacyDrawing r:id="rId259"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId261"/>
+  <legacyDrawing r:id="rId262"/>
 </worksheet>
 </file>
</xml_diff>